<commit_message>
updated code and some data files
</commit_message>
<xml_diff>
--- a/data/BBMB_ClueTestLocations.xlsx
+++ b/data/BBMB_ClueTestLocations.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\Workspace\ClueGameBBMB\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6240"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="BBMB_ClueLayout.csv" sheetId="1" r:id="rId3"/>
+    <sheet name="BBMB_ClueLayout.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -109,21 +117,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -210,93 +221,343 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="2.71"/>
-    <col customWidth="1" min="5" max="5" width="3.71"/>
-    <col customWidth="1" min="6" max="6" width="3.86"/>
-    <col customWidth="1" min="7" max="8" width="3.57"/>
-    <col customWidth="1" min="9" max="9" width="2.71"/>
-    <col customWidth="1" min="10" max="10" width="3.57"/>
-    <col customWidth="1" min="11" max="13" width="2.71"/>
-    <col customWidth="1" min="14" max="14" width="3.57"/>
-    <col customWidth="1" min="15" max="16" width="2.71"/>
-    <col customWidth="1" min="17" max="17" width="3.86"/>
-    <col customWidth="1" min="18" max="18" width="2.71"/>
-    <col customWidth="1" min="19" max="19" width="3.57"/>
-    <col customWidth="1" min="20" max="20" width="3.43"/>
-    <col customWidth="1" min="21" max="21" width="2.71"/>
-    <col customWidth="1" min="22" max="22" width="3.86"/>
-    <col customWidth="1" min="23" max="23" width="2.71"/>
+    <col min="1" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="8" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="13" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" customWidth="1"/>
+    <col min="15" max="16" width="2.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" customWidth="1"/>
+    <col min="19" max="19" width="3.5703125" customWidth="1"/>
+    <col min="20" max="20" width="3.42578125" customWidth="1"/>
+    <col min="21" max="21" width="2.7109375" customWidth="1"/>
+    <col min="22" max="22" width="3.85546875" customWidth="1"/>
+    <col min="23" max="23" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -367,7 +628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -438,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -509,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -580,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -651,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -722,7 +983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,7 +1054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -864,7 +1125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -935,7 +1196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1006,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1077,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1408,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>15</v>
@@ -1432,7 +1693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1503,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1574,7 +1835,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1645,7 +1906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1716,7 +1977,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -1787,7 +2048,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
@@ -1858,22 +2119,46 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="11" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="10" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>26</v>
       </c>
@@ -1886,36 +2171,68 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="8" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
         <v>30</v>
       </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A24:I24"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="A28:I28"/>
     <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A31:I31"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>